<commit_message>
ajout quete + correction point/indice
</commit_message>
<xml_diff>
--- a/Quete/Taverne3.xlsx
+++ b/Quete/Taverne3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D154B5-8651-479E-B6FF-561793C2C078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8593E8-2CF0-4601-968E-CC0D0F9635F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
   <si>
     <t>Chap</t>
   </si>
@@ -117,6 +117,215 @@
   </si>
   <si>
     <t>Pentagone</t>
+  </si>
+  <si>
+    <t>Triangle X</t>
+  </si>
+  <si>
+    <t>x
+xx
+xxx
+xxxx
+xxxxx
+xxxxxx
+xxxxxxx
+xxxxxxxx
+xxxxxxxxx</t>
+  </si>
+  <si>
+    <t>x
+xx
+xxx
+xxxx
+xxxxx
+xxxxxx
+xxxxxxx</t>
+  </si>
+  <si>
+    <t>x
+xx</t>
+  </si>
+  <si>
+    <t>x
+xx
+xxx
+xxxx</t>
+  </si>
+  <si>
+    <t>Ecriver un programme permettant d'afficher des triangles fait de 'x' vu comme dans les output d'exemple</t>
+  </si>
+  <si>
+    <t>x
+xx
+xxx
+xxxx
+xxxxx
+xxxxxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecrivez la boucle ‘for’ qui permette l’affichage de :
+a) 0 1 2 3 4
+b) 1 4 9 16 25
+c) 2 4 6 8 
+d) 10 9 8 7 6
+Le format des inputs est defini comme ceci
+la 1ere ligne est une lettre correspondant au type de suite
+la 2eme ligne consiste au nombre d'element qui sont dans la suite </t>
+  </si>
+  <si>
+    <t>Suite easy</t>
+  </si>
+  <si>
+    <t>Suite medium</t>
+  </si>
+  <si>
+    <t>a
+6</t>
+  </si>
+  <si>
+    <t>1
+1
+2
+3
+5
+8
+13</t>
+  </si>
+  <si>
+    <t>b
+4</t>
+  </si>
+  <si>
+    <t>1
+3
+6
+10</t>
+  </si>
+  <si>
+    <t>7
+22
+11
+34
+17</t>
+  </si>
+  <si>
+    <t>c
+5</t>
+  </si>
+  <si>
+    <t>0
+1
+2
+3
+4
+5</t>
+  </si>
+  <si>
+    <t>1
+4
+9
+16</t>
+  </si>
+  <si>
+    <t>d
+3</t>
+  </si>
+  <si>
+    <t>10
+9
+8</t>
+  </si>
+  <si>
+    <t>b
+8</t>
+  </si>
+  <si>
+    <t>1
+4
+9
+16
+25
+36
+49
+64</t>
+  </si>
+  <si>
+    <t>d
+9</t>
+  </si>
+  <si>
+    <t>10
+9
+8
+7
+6
+5
+4
+3
+2</t>
+  </si>
+  <si>
+    <t>2
+4
+6
+8
+10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecrivez la boucle ‘for’ qui permette l’affichage de :
+a) 1 3 6 10 15
+b) 1 1 2 3 5 8 13 21 
+c)  7 22 11 34 17 52 26 13
+Le format des inputs est defini comme ceci
+la 1ere ligne est une lettre correspondant au type de suite
+la 2eme ligne consiste au nombre d'element qui sont dans la suite </t>
+  </si>
+  <si>
+    <t>a
+4</t>
+  </si>
+  <si>
+    <t>b
+7</t>
+  </si>
+  <si>
+    <t>1
+1
+2
+3
+5
+8
+13
+21
+34
+55
+89
+144
+233</t>
+  </si>
+  <si>
+    <t>b
+13</t>
+  </si>
+  <si>
+    <t>c
+15</t>
+  </si>
+  <si>
+    <t>1
+3
+6
+10
+15
+21
+28
+36
+45
+55</t>
+  </si>
+  <si>
+    <t>a
+10</t>
   </si>
 </sst>
 </file>
@@ -502,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="93" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="93" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,7 +814,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1">
@@ -662,58 +871,196 @@
       </c>
     </row>
     <row r="3" spans="1:25" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1">
+        <v>7</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
+      <c r="Q3" s="1">
+        <v>3</v>
+      </c>
+      <c r="R3" s="1">
+        <v>2</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="1">
+        <v>9</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V3" s="1">
+        <v>6</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="2"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+    <row r="4" spans="1:25" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
+      <c r="Q4" s="1">
+        <v>4</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="360" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>4</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
@@ -721,11 +1068,9 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>

</xml_diff>

<commit_message>
Correction nom de variable
</commit_message>
<xml_diff>
--- a/Quete/Taverne3.xlsx
+++ b/Quete/Taverne3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Python_Apprendre_Autrement\Quete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493F4724-B1E5-4B1A-9B7A-B9996AF94096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15870F87-8A37-4004-A8C4-133DF0CE24DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="348" windowWidth="17280" windowHeight="9420" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CA7E0B7-CDFC-4FD5-BEF9-F0FFA02D3C1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -163,16 +163,6 @@
 xxxxxx</t>
   </si>
   <si>
-    <t xml:space="preserve">Ecrivez la boucle ‘for’ qui permette l’affichage de :
-a) 0 1 2 3 4
-b) 1 4 9 16 25
-c) 2 4 6 8 
-d) 10 9 8 7 6
-Le format des inputs est defini comme ceci
-la 1ere ligne est une lettre correspondant au type de suite
-la 2eme ligne consiste au nombre d'element qui sont dans la suite </t>
-  </si>
-  <si>
     <t>Suite easy</t>
   </si>
   <si>
@@ -270,15 +260,6 @@
 6
 8
 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ecrivez la boucle ‘for’ qui permette l’affichage de :
-a) 1 3 6 10 15
-b) 1 1 2 3 5 8 13 21 
-c)  7 22 11 34 17 52 26 13
-Le format des inputs est defini comme ceci
-la 1ere ligne est une lettre correspondant au type de suite
-la 2eme ligne consiste au nombre d'element qui sont dans la suite </t>
   </si>
   <si>
     <t>a
@@ -326,6 +307,25 @@
   <si>
     <t>a
 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecrivez la boucle ‘for’ qui permette l’affichage de :
+a) 1 3 6 10 15 ...
+b) 1 1 2 3 5 8 13 21 ...
+c)  7 22 11 34 17 52 26 13 ...
+Le format des inputs est defini comme ceci
+la 1ere ligne est une lettre correspondant au type de suite
+la 2eme ligne consiste au nombre d'element qui sont dans la suite </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ecrivez la boucle ‘for’ qui permette l’affichage de :
+a) 0 1 2 3 4 ...
+b) 1 4 9 16 25 ...
+c) 2 4 6 8 ... 
+d) 10 9 8 7 6 ...
+Le format des inputs est defini comme ceci
+la 1ere ligne est une lettre correspondant au type de suite
+la 2eme ligne consiste au nombre d'element qui sont dans la suite </t>
   </si>
 </sst>
 </file>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F0EE0D-D391-4AA7-AF3E-FA9E64764AC4}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -933,12 +933,12 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="2"/>
     </row>
-    <row r="4" spans="1:25" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -948,25 +948,25 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -976,36 +976,36 @@
         <v>4</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="X4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="X4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>51</v>
-      </c>
     </row>
-    <row r="5" spans="1:25" ht="360" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -1014,52 +1014,52 @@
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="Q5" s="1">
         <v>4</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T5" s="1" t="s">
+      <c r="V5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y5" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">

</xml_diff>